<commit_message>
Fixing issue with XlsReader and xlsx test file
</commit_message>
<xml_diff>
--- a/Test/Files/test.xlsx
+++ b/Test/Files/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="18195" windowHeight="12585"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="5">
   <si>
-    <t>Headers</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
     <t>This</t>
   </si>
   <si>
@@ -31,6 +25,12 @@
   </si>
   <si>
     <t>My</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -365,23 +365,23 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D13"/>
+      <selection activeCell="B2" sqref="B2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -389,13 +389,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -403,13 +403,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -417,13 +417,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -431,13 +431,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -445,13 +445,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -459,13 +459,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -473,13 +473,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -487,13 +487,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -501,13 +501,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -515,13 +515,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -529,13 +529,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -543,13 +543,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>